<commit_message>
Included sample jxls query with chart in demo database
</commit_message>
<xml_diff>
--- a/art/src/art/WEB-INF/templates/sample-jxls2.xlsx
+++ b/art/src/art/WEB-INF/templates/sample-jxls2.xlsx
@@ -48,22 +48,22 @@
     <t>Volume</t>
   </si>
   <si>
-    <t>results</t>
-  </si>
-  <si>
     <t>${results.ORDER_ID}</t>
   </si>
   <si>
     <t>${results.CITY_NAME}</t>
   </si>
   <si>
-    <t>${results.results_NAME}</t>
-  </si>
-  <si>
     <t>${results.ORDER_DATE}</t>
   </si>
   <si>
     <t>${results.VOLUME}</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>${results.ITEM_NAME}</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +496,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
@@ -507,19 +507,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F10" s="1"/>
     </row>

</xml_diff>